<commit_message>
newest cytometer data analysis files
</commit_message>
<xml_diff>
--- a/META_cyto.xlsx
+++ b/META_cyto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/alanna_leale_wur_nl/Documents/2023_montpellier/experiments/cytometer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/alanna_leale_wur_nl/Documents/2023_montpellier/experiments/data/cytometer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="8_{18EF97E1-74D5-7241-9D12-5FEF4C951DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{088BC86B-BA99-EA45-A10D-09833D9164A3}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="8_{18EF97E1-74D5-7241-9D12-5FEF4C951DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{068A9F18-4AB6-9344-97F3-979C4CB68743}"/>
   <bookViews>
     <workbookView xWindow="30080" yWindow="500" windowWidth="31060" windowHeight="19020" xr2:uid="{33AE3A6E-CACA-F94E-92F1-C15C36CBBBA0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="36">
   <si>
     <t>comm</t>
   </si>
@@ -141,13 +141,16 @@
   </si>
   <si>
     <t>r04</t>
+  </si>
+  <si>
+    <t>richness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,14 +160,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,6 +192,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -218,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -241,19 +242,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,19 +586,19 @@
   <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="3.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -620,12 +635,15 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C2">
@@ -646,24 +664,27 @@
       <c r="H2">
         <v>200</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C3">
@@ -684,24 +705,27 @@
       <c r="H3">
         <v>200</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="I3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C4">
@@ -722,24 +746,27 @@
       <c r="H4">
         <v>200</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C5">
@@ -760,24 +787,27 @@
       <c r="H5">
         <v>200</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="I5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C6">
@@ -798,24 +828,27 @@
       <c r="H6">
         <v>200</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C7">
@@ -836,24 +869,27 @@
       <c r="H7">
         <v>200</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C8">
@@ -874,24 +910,27 @@
       <c r="H8">
         <v>200</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="I8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C9">
@@ -912,24 +951,27 @@
       <c r="H9">
         <v>200</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="I9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C10">
@@ -950,24 +992,27 @@
       <c r="H10">
         <v>200</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="I10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11">
@@ -988,24 +1033,27 @@
       <c r="H11">
         <v>200</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="I11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C12">
@@ -1026,30 +1074,33 @@
       <c r="H12">
         <v>200</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="I12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>10</v>
       </c>
       <c r="E13" s="2">
@@ -1064,24 +1115,27 @@
       <c r="H13">
         <v>200</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="I13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C14">
@@ -1102,24 +1156,27 @@
       <c r="H14">
         <v>200</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="I14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C15">
@@ -1140,24 +1197,27 @@
       <c r="H15">
         <v>200</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="I15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C16">
@@ -1178,24 +1238,27 @@
       <c r="H16">
         <v>200</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="I16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C17">
@@ -1216,24 +1279,27 @@
       <c r="H17">
         <v>200</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="I17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C18">
@@ -1254,20 +1320,23 @@
       <c r="H18">
         <v>200</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="I18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1292,20 +1361,23 @@
       <c r="H19">
         <v>200</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="I19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1330,20 +1402,23 @@
       <c r="H20">
         <v>200</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="I20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1368,20 +1443,23 @@
       <c r="H21">
         <v>200</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="I21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1406,20 +1484,23 @@
       <c r="H22">
         <v>200</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="I22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1444,20 +1525,23 @@
       <c r="H23">
         <v>200</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="I23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1482,20 +1566,23 @@
       <c r="H24">
         <v>200</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="I24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1520,20 +1607,23 @@
       <c r="H25">
         <v>200</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="I25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1558,20 +1648,23 @@
       <c r="H26">
         <v>200</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="I26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1596,20 +1689,23 @@
       <c r="H27">
         <v>200</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="I27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1634,20 +1730,23 @@
       <c r="H28">
         <v>200</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="I28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1672,20 +1771,23 @@
       <c r="H29">
         <v>200</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="I29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M29" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1710,20 +1812,23 @@
       <c r="H30">
         <v>200</v>
       </c>
-      <c r="I30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="I30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M30" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1748,20 +1853,23 @@
       <c r="H31">
         <v>200</v>
       </c>
-      <c r="I31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="I31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -1786,20 +1894,23 @@
       <c r="H32">
         <v>200</v>
       </c>
-      <c r="I32" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="I32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M32" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1824,20 +1935,23 @@
       <c r="H33">
         <v>200</v>
       </c>
-      <c r="I33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="I33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1862,20 +1976,23 @@
       <c r="H34">
         <v>200</v>
       </c>
-      <c r="I34" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="I34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M34" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -1900,24 +2017,27 @@
       <c r="H35">
         <v>200</v>
       </c>
-      <c r="I35" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="I35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M35" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C36">
@@ -1938,25 +2058,27 @@
       <c r="H36">
         <v>200</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L36" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M36" s="3"/>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="I36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C37">
@@ -1977,25 +2099,27 @@
       <c r="H37">
         <v>200</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="I37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M37" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C38">
@@ -2016,25 +2140,27 @@
       <c r="H38">
         <v>200</v>
       </c>
-      <c r="I38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L38" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="I38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M38" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C39">
@@ -2055,25 +2181,27 @@
       <c r="H39">
         <v>200</v>
       </c>
-      <c r="I39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M39" s="3"/>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="I39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M39" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C40">
@@ -2094,25 +2222,27 @@
       <c r="H40">
         <v>200</v>
       </c>
-      <c r="I40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M40" s="3"/>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="I40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M40" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C41">
@@ -2133,25 +2263,27 @@
       <c r="H41">
         <v>200</v>
       </c>
-      <c r="I41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="I41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M41" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C42">
@@ -2172,25 +2304,27 @@
       <c r="H42">
         <v>200</v>
       </c>
-      <c r="I42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K42" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M42" s="3"/>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="I42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M42" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C43">
@@ -2211,25 +2345,27 @@
       <c r="H43">
         <v>200</v>
       </c>
-      <c r="I43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M43" s="3"/>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="I43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M43" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C44">
@@ -2250,25 +2386,27 @@
       <c r="H44">
         <v>200</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M44" s="3"/>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="I44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M44" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C45">
@@ -2289,25 +2427,27 @@
       <c r="H45">
         <v>200</v>
       </c>
-      <c r="I45" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L45" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M45" s="3"/>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="I45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M45" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>25</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C46">
@@ -2328,31 +2468,33 @@
       <c r="H46">
         <v>200</v>
       </c>
-      <c r="I46" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M46" s="3"/>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="I46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M46" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <v>10</v>
       </c>
       <c r="E47" s="2">
@@ -2367,25 +2509,27 @@
       <c r="H47">
         <v>200</v>
       </c>
-      <c r="I47" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L47" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M47" s="3"/>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="I47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M47" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C48">
@@ -2406,25 +2550,27 @@
       <c r="H48">
         <v>200</v>
       </c>
-      <c r="I48" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K48" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M48" s="3"/>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="I48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M48" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C49">
@@ -2445,25 +2591,27 @@
       <c r="H49">
         <v>200</v>
       </c>
-      <c r="I49" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K49" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L49" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M49" s="3"/>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="I49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M49" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C50">
@@ -2484,25 +2632,27 @@
       <c r="H50">
         <v>200</v>
       </c>
-      <c r="I50" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K50" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M50" s="3"/>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="I50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M50" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C51">
@@ -2523,25 +2673,27 @@
       <c r="H51">
         <v>200</v>
       </c>
-      <c r="I51" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J51" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M51" s="3"/>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="I51" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M51" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C52">
@@ -2562,21 +2714,23 @@
       <c r="H52">
         <v>200</v>
       </c>
-      <c r="I52" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M52" s="3"/>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="I52" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M52" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2595,21 +2749,29 @@
       <c r="F53">
         <v>200</v>
       </c>
-      <c r="I53" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J53" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K53" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L53" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M53" s="3"/>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="G53">
+        <v>200</v>
+      </c>
+      <c r="H53">
+        <v>200</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M53" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -2628,20 +2790,29 @@
       <c r="F54">
         <v>200</v>
       </c>
-      <c r="I54" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K54" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L54" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="G54">
+        <v>200</v>
+      </c>
+      <c r="H54">
+        <v>200</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M54" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -2660,20 +2831,29 @@
       <c r="F55">
         <v>200</v>
       </c>
-      <c r="I55" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L55" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="G55">
+        <v>200</v>
+      </c>
+      <c r="H55">
+        <v>200</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M55" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2692,20 +2872,29 @@
       <c r="F56">
         <v>200</v>
       </c>
-      <c r="I56" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K56" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L56" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="G56">
+        <v>200</v>
+      </c>
+      <c r="H56">
+        <v>200</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M56" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2724,20 +2913,29 @@
       <c r="F57">
         <v>200</v>
       </c>
-      <c r="I57" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L57" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="G57">
+        <v>200</v>
+      </c>
+      <c r="H57">
+        <v>200</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M57" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -2756,20 +2954,29 @@
       <c r="F58">
         <v>200</v>
       </c>
-      <c r="I58" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L58" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="G58">
+        <v>200</v>
+      </c>
+      <c r="H58">
+        <v>200</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L58" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M58" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>21</v>
       </c>
@@ -2788,20 +2995,29 @@
       <c r="F59">
         <v>200</v>
       </c>
-      <c r="I59" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K59" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L59" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="G59">
+        <v>200</v>
+      </c>
+      <c r="H59">
+        <v>200</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K59" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M59" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>22</v>
       </c>
@@ -2820,20 +3036,29 @@
       <c r="F60">
         <v>200</v>
       </c>
-      <c r="I60" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L60" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="G60">
+        <v>200</v>
+      </c>
+      <c r="H60">
+        <v>200</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M60" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -2852,20 +3077,29 @@
       <c r="F61">
         <v>200</v>
       </c>
-      <c r="I61" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L61" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="G61">
+        <v>200</v>
+      </c>
+      <c r="H61">
+        <v>200</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M61" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -2884,20 +3118,29 @@
       <c r="F62">
         <v>200</v>
       </c>
-      <c r="I62" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J62" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K62" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L62" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="G62">
+        <v>200</v>
+      </c>
+      <c r="H62">
+        <v>200</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M62" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>25</v>
       </c>
@@ -2916,20 +3159,29 @@
       <c r="F63">
         <v>200</v>
       </c>
-      <c r="I63" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K63" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L63" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="G63">
+        <v>200</v>
+      </c>
+      <c r="H63">
+        <v>200</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M63" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -2939,7 +3191,7 @@
       <c r="C64">
         <v>3</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="6">
         <v>10</v>
       </c>
       <c r="E64" s="2">
@@ -2948,20 +3200,29 @@
       <c r="F64">
         <v>200</v>
       </c>
-      <c r="I64" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K64" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L64" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="G64">
+        <v>200</v>
+      </c>
+      <c r="H64">
+        <v>200</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L64" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M64" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>27</v>
       </c>
@@ -2980,21 +3241,29 @@
       <c r="F65">
         <v>200</v>
       </c>
-      <c r="G65" s="2"/>
-      <c r="I65" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K65" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L65" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="G65" s="2">
+        <v>100</v>
+      </c>
+      <c r="H65">
+        <v>200</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L65" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M65" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -3013,20 +3282,29 @@
       <c r="F66">
         <v>200</v>
       </c>
-      <c r="I66" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J66" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L66" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="G66">
+        <v>200</v>
+      </c>
+      <c r="H66">
+        <v>200</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M66" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>29</v>
       </c>
@@ -3045,20 +3323,29 @@
       <c r="F67">
         <v>200</v>
       </c>
-      <c r="I67" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K67" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L67" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="G67">
+        <v>200</v>
+      </c>
+      <c r="H67">
+        <v>200</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M67" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>30</v>
       </c>
@@ -3077,21 +3364,29 @@
       <c r="F68">
         <v>200</v>
       </c>
-      <c r="G68" s="2"/>
-      <c r="I68" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K68" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L68" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="G68" s="2">
+        <v>100</v>
+      </c>
+      <c r="H68">
+        <v>200</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M68" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>31</v>
       </c>
@@ -3110,17 +3405,26 @@
       <c r="F69">
         <v>200</v>
       </c>
-      <c r="I69" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J69" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K69" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L69" s="4" t="s">
-        <v>14</v>
+      <c r="G69">
+        <v>200</v>
+      </c>
+      <c r="H69">
+        <v>200</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M69" s="8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>